<commit_message>
HeRE: Data and Processing
Files which begin to analyse the data from worldwide surveys to estimate the hesitance and resistance per age group,
</commit_message>
<xml_diff>
--- a/Hesitance_Resistance_Modelling/COVID_Vaccine_HesitanceResistance_QLD_Stats.xlsx
+++ b/Hesitance_Resistance_Modelling/COVID_Vaccine_HesitanceResistance_QLD_Stats.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lachlanHa\Downloads\Hesitance_Resistance_Modelling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uq-my.sharepoint.com/personal/uqlhami6_uq_edu_au/Documents/pHonours/QIMRB/covid-ra-sandbox/Hesitance_Resistance_Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_C146B534B62CCB6ED5862D4553907CDC6AA00322" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{05BD4B62-914C-48D8-B41D-CF388C75D058}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="2" r:id="rId1"/>
@@ -102,9 +103,6 @@
     <t>Note: Age categories will be merged if data doesn't contain date</t>
   </si>
   <si>
-    <t>(e.g. if only 11-20, then 20-24 and 25-29 will share value)</t>
-  </si>
-  <si>
     <t xml:space="preserve">DSV = Data source value </t>
   </si>
   <si>
@@ -157,12 +155,15 @@
   </si>
   <si>
     <t xml:space="preserve">Some had qualitative scales (completely disagree, somewhat disagree, neutral, somewhat agree, completely agree). Because getting vaccinated is an active choice, disagree/neutral counts as hesitant </t>
+  </si>
+  <si>
+    <t>(e.g. if only 20-30, then 20-24 and 25-29 will share value)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -495,11 +496,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,27 +530,27 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -558,11 +559,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,10 +576,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -644,16 +645,16 @@
         <v>20</v>
       </c>
       <c r="X1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA1" t="s">
         <v>27</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -661,20 +662,20 @@
         <v>44044</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W2" s="3"/>
       <c r="X2">
         <v>3</v>
       </c>
       <c r="Y2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Z2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AA2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -682,20 +683,20 @@
         <v>44044</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W3" s="3"/>
       <c r="X3">
         <v>2</v>
       </c>
       <c r="Y3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Z3" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="AA3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>